<commit_message>
Update request, search, notification
</commit_message>
<xml_diff>
--- a/invoices-02_2025.xlsx
+++ b/invoices-02_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\BuildingManagerPTIT-APP\PTIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E438DAA-0953-427B-ABD9-24E7D5B77CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E83CCA-2935-42D8-B9DB-9587A63E4D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -305,10 +305,10 @@
     <t>Unit 648</t>
   </si>
   <si>
-    <t>02/2025</t>
-  </si>
-  <si>
     <t>current Number</t>
+  </si>
+  <si>
+    <t>03/2025</t>
   </si>
 </sst>
 </file>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,11 +714,11 @@
         <v>25000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(7, 10)</f>
-        <v>8</v>
+        <f ca="1">RANDBETWEEN(11, 14)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -729,11 +729,11 @@
         <v>25000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" ca="1" si="0">RANDBETWEEN(7, 10)</f>
-        <v>10</v>
+        <f t="shared" ref="D3:D66" ca="1" si="0">RANDBETWEEN(11, 14)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -744,11 +744,11 @@
         <v>25000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -759,11 +759,11 @@
         <v>25000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -774,11 +774,11 @@
         <v>25000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -789,11 +789,11 @@
         <v>25000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -804,11 +804,11 @@
         <v>25000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -819,11 +819,11 @@
         <v>25000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -834,11 +834,11 @@
         <v>25000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -849,11 +849,11 @@
         <v>25000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -864,11 +864,11 @@
         <v>25000</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -879,11 +879,11 @@
         <v>25000</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -894,11 +894,11 @@
         <v>25000</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -909,11 +909,11 @@
         <v>25000</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -924,11 +924,11 @@
         <v>25000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -939,11 +939,11 @@
         <v>25000</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -954,11 +954,11 @@
         <v>25000</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -969,11 +969,11 @@
         <v>25000</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -984,11 +984,11 @@
         <v>25000</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -999,11 +999,11 @@
         <v>25000</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1014,11 +1014,11 @@
         <v>25000</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1029,11 +1029,11 @@
         <v>25000</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1044,11 +1044,11 @@
         <v>25000</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1059,11 +1059,11 @@
         <v>25000</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1074,11 +1074,11 @@
         <v>25000</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1089,11 +1089,11 @@
         <v>25000</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1104,11 +1104,11 @@
         <v>25000</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1119,11 +1119,11 @@
         <v>25000</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1134,11 +1134,11 @@
         <v>25000</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1149,11 +1149,11 @@
         <v>25000</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1164,11 +1164,11 @@
         <v>25000</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1179,11 +1179,11 @@
         <v>25000</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1194,11 +1194,11 @@
         <v>25000</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1209,11 +1209,11 @@
         <v>25000</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1224,11 +1224,11 @@
         <v>25000</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1239,11 +1239,11 @@
         <v>25000</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1254,11 +1254,11 @@
         <v>25000</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1269,11 +1269,11 @@
         <v>25000</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1284,11 +1284,11 @@
         <v>25000</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1299,11 +1299,11 @@
         <v>25000</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1314,11 +1314,11 @@
         <v>25000</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1329,11 +1329,11 @@
         <v>25000</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1344,11 +1344,11 @@
         <v>25000</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1359,11 +1359,11 @@
         <v>25000</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1374,11 +1374,11 @@
         <v>25000</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1389,11 +1389,11 @@
         <v>25000</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1404,11 +1404,11 @@
         <v>25000</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1419,11 +1419,11 @@
         <v>25000</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1434,11 +1434,11 @@
         <v>25000</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1449,11 +1449,11 @@
         <v>25000</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1464,11 +1464,11 @@
         <v>25000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1479,11 +1479,11 @@
         <v>25000</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1494,11 +1494,11 @@
         <v>25000</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,11 +1509,11 @@
         <v>25000</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1524,11 +1524,11 @@
         <v>25000</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1539,11 +1539,11 @@
         <v>25000</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1554,11 +1554,11 @@
         <v>25000</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1569,11 +1569,11 @@
         <v>25000</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1584,11 +1584,11 @@
         <v>25000</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1599,11 +1599,11 @@
         <v>25000</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1614,11 +1614,11 @@
         <v>25000</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1629,11 +1629,11 @@
         <v>25000</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1644,11 +1644,11 @@
         <v>25000</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,11 +1659,11 @@
         <v>25000</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1674,11 +1674,11 @@
         <v>25000</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1689,11 +1689,11 @@
         <v>25000</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D91" ca="1" si="1">RANDBETWEEN(7, 10)</f>
-        <v>10</v>
+        <f t="shared" ref="D67:D91" ca="1" si="1">RANDBETWEEN(11, 14)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,11 +1704,11 @@
         <v>25000</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1719,11 +1719,11 @@
         <v>25000</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1734,11 +1734,11 @@
         <v>25000</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1749,11 +1749,11 @@
         <v>25000</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1764,11 +1764,11 @@
         <v>25000</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1779,11 +1779,11 @@
         <v>25000</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1794,11 +1794,11 @@
         <v>25000</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1809,11 +1809,11 @@
         <v>25000</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1824,11 +1824,11 @@
         <v>25000</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1839,11 +1839,11 @@
         <v>25000</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1854,11 +1854,11 @@
         <v>25000</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1869,11 +1869,11 @@
         <v>25000</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1884,11 +1884,11 @@
         <v>25000</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1899,11 +1899,11 @@
         <v>25000</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,11 +1914,11 @@
         <v>25000</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1929,11 +1929,11 @@
         <v>25000</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1944,11 +1944,11 @@
         <v>25000</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1959,11 +1959,11 @@
         <v>25000</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1974,11 +1974,11 @@
         <v>25000</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1989,11 +1989,11 @@
         <v>25000</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2004,11 +2004,11 @@
         <v>25000</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2019,11 +2019,11 @@
         <v>25000</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2034,11 +2034,11 @@
         <v>25000</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2049,11 +2049,11 @@
         <v>25000</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2066,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2089,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2100,11 +2100,11 @@
         <v>3500</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(51, 70)</f>
-        <v>58</v>
+        <f ca="1">RANDBETWEEN(71, 80)</f>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2115,11 +2115,11 @@
         <v>3500</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" ca="1" si="0">RANDBETWEEN(51, 70)</f>
-        <v>68</v>
+        <f t="shared" ref="D3:D66" ca="1" si="0">RANDBETWEEN(71, 80)</f>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2130,11 +2130,11 @@
         <v>3500</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2145,11 +2145,11 @@
         <v>3500</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2160,11 +2160,11 @@
         <v>3500</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2175,11 +2175,11 @@
         <v>3500</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2190,11 +2190,11 @@
         <v>3500</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2205,11 +2205,11 @@
         <v>3500</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -2220,11 +2220,11 @@
         <v>3500</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -2235,11 +2235,11 @@
         <v>3500</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2250,11 +2250,11 @@
         <v>3500</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2265,11 +2265,11 @@
         <v>3500</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2280,11 +2280,11 @@
         <v>3500</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2295,11 +2295,11 @@
         <v>3500</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2310,11 +2310,11 @@
         <v>3500</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2325,11 +2325,11 @@
         <v>3500</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2340,11 +2340,11 @@
         <v>3500</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2355,11 +2355,11 @@
         <v>3500</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2370,11 +2370,11 @@
         <v>3500</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2385,11 +2385,11 @@
         <v>3500</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2400,11 +2400,11 @@
         <v>3500</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2415,11 +2415,11 @@
         <v>3500</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -2430,11 +2430,11 @@
         <v>3500</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2445,11 +2445,11 @@
         <v>3500</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2460,11 +2460,11 @@
         <v>3500</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2475,11 +2475,11 @@
         <v>3500</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2490,11 +2490,11 @@
         <v>3500</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2505,11 +2505,11 @@
         <v>3500</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2520,11 +2520,11 @@
         <v>3500</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2535,11 +2535,11 @@
         <v>3500</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2550,11 +2550,11 @@
         <v>3500</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2565,11 +2565,11 @@
         <v>3500</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2580,11 +2580,11 @@
         <v>3500</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -2595,11 +2595,11 @@
         <v>3500</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2610,11 +2610,11 @@
         <v>3500</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -2625,11 +2625,11 @@
         <v>3500</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2640,11 +2640,11 @@
         <v>3500</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2655,11 +2655,11 @@
         <v>3500</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2670,11 +2670,11 @@
         <v>3500</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -2685,11 +2685,11 @@
         <v>3500</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2700,11 +2700,11 @@
         <v>3500</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2715,11 +2715,11 @@
         <v>3500</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2730,11 +2730,11 @@
         <v>3500</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2745,11 +2745,11 @@
         <v>3500</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2760,11 +2760,11 @@
         <v>3500</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2775,11 +2775,11 @@
         <v>3500</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2790,11 +2790,11 @@
         <v>3500</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2805,11 +2805,11 @@
         <v>3500</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2820,11 +2820,11 @@
         <v>3500</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2835,11 +2835,11 @@
         <v>3500</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2850,11 +2850,11 @@
         <v>3500</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2865,11 +2865,11 @@
         <v>3500</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2880,11 +2880,11 @@
         <v>3500</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2895,11 +2895,11 @@
         <v>3500</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2910,11 +2910,11 @@
         <v>3500</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2925,11 +2925,11 @@
         <v>3500</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2940,11 +2940,11 @@
         <v>3500</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2955,11 +2955,11 @@
         <v>3500</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2970,11 +2970,11 @@
         <v>3500</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2985,11 +2985,11 @@
         <v>3500</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -3000,11 +3000,11 @@
         <v>3500</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -3015,11 +3015,11 @@
         <v>3500</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -3030,11 +3030,11 @@
         <v>3500</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3045,11 +3045,11 @@
         <v>3500</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -3060,11 +3060,11 @@
         <v>3500</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3075,11 +3075,11 @@
         <v>3500</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D91" ca="1" si="1">RANDBETWEEN(51, 70)</f>
-        <v>56</v>
+        <f t="shared" ref="D67:D91" ca="1" si="1">RANDBETWEEN(71, 80)</f>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3090,11 +3090,11 @@
         <v>3500</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3105,11 +3105,11 @@
         <v>3500</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="1"/>
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -3120,11 +3120,11 @@
         <v>3500</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -3135,11 +3135,11 @@
         <v>3500</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="1"/>
-        <v>66</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -3150,11 +3150,11 @@
         <v>3500</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -3165,11 +3165,11 @@
         <v>3500</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -3180,11 +3180,11 @@
         <v>3500</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -3195,11 +3195,11 @@
         <v>3500</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="1"/>
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -3210,11 +3210,11 @@
         <v>3500</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -3225,11 +3225,11 @@
         <v>3500</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -3240,11 +3240,11 @@
         <v>3500</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -3255,11 +3255,11 @@
         <v>3500</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3270,11 +3270,11 @@
         <v>3500</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -3285,11 +3285,11 @@
         <v>3500</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="1"/>
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -3300,11 +3300,11 @@
         <v>3500</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -3315,11 +3315,11 @@
         <v>3500</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -3330,11 +3330,11 @@
         <v>3500</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -3345,11 +3345,11 @@
         <v>3500</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="1"/>
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3360,11 +3360,11 @@
         <v>3500</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -3375,11 +3375,11 @@
         <v>3500</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="1"/>
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -3390,11 +3390,11 @@
         <v>3500</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D88">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3405,11 +3405,11 @@
         <v>3500</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="1"/>
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -3420,11 +3420,11 @@
         <v>3500</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -3435,11 +3435,11 @@
         <v>3500</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>